<commit_message>
✨ Récupération du classement | Documentation
</commit_message>
<xml_diff>
--- a/00 - Documents/2_PASCHE_Planning_2023.xlsx
+++ b/00 - Documents/2_PASCHE_Planning_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paschek7/TPI/futnetsinglemaster/00 - Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772FA13F-4A76-6A4A-8ADB-588E8A221AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D6A7C9-7FA4-9F44-AC39-6D86963DBBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="8" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="49">
   <si>
     <t>Tâches</t>
   </si>
@@ -1557,11 +1557,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CN39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="R11" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="BC15" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AQ22" sqref="AQ22"/>
+      <selection pane="bottomRight" activeCell="BO19" sqref="BO19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3631,12 +3631,24 @@
       <c r="BI19" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="BJ19" s="31"/>
-      <c r="BK19" s="31"/>
-      <c r="BL19" s="31"/>
-      <c r="BM19" s="31"/>
-      <c r="BN19" s="31"/>
-      <c r="BO19" s="31"/>
+      <c r="BJ19" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="BK19" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="BL19" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="BM19" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="BN19" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="BO19" s="31" t="s">
+        <v>41</v>
+      </c>
       <c r="BP19" s="31"/>
       <c r="BQ19" s="31"/>
       <c r="BR19" s="31"/>
@@ -4634,7 +4646,9 @@
       <c r="BL29" s="38"/>
       <c r="BM29" s="38"/>
       <c r="BN29" s="38"/>
-      <c r="BO29" s="33"/>
+      <c r="BO29" s="33" t="s">
+        <v>41</v>
+      </c>
       <c r="BP29" s="40"/>
       <c r="BQ29" s="38"/>
       <c r="BR29" s="38"/>

</xml_diff>